<commit_message>
next steps: compare measurements
</commit_message>
<xml_diff>
--- a/Zhuang-sumstats.xlsx
+++ b/Zhuang-sumstats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://colostate-my.sharepoint.com/personal/khobbs01_colostate_edu/Documents/Desktop/Dissertation/headscan_dissertation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7EB40DF8-F07A-4E27-8B6F-FD95CA7BB173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{7EB40DF8-F07A-4E27-8B6F-FD95CA7BB173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A67C5CB4-354B-4D78-A40C-6C109AB08DF1}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{B38B8ADD-B645-4C66-B316-0CE56ADDA135}"/>
   </bookViews>
@@ -104,43 +104,43 @@
     <t xml:space="preserve">Weight </t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Mean</t>
-  </si>
-  <si>
-    <t>SD</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
     <t>Female</t>
   </si>
   <si>
-    <t>5th</t>
-  </si>
-  <si>
-    <t>25th</t>
-  </si>
-  <si>
-    <t>50th</t>
-  </si>
-  <si>
-    <t>75th</t>
-  </si>
-  <si>
-    <t>95th</t>
+    <t>percent5th</t>
+  </si>
+  <si>
+    <t>percent25th</t>
+  </si>
+  <si>
+    <t>percent50th</t>
+  </si>
+  <si>
+    <t>percent75th</t>
+  </si>
+  <si>
+    <t>percent95th</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sd</t>
   </si>
 </sst>
 </file>
@@ -494,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C212D599-0EF9-4878-A52E-653D095A5BBB}">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -508,37 +508,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="I1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="L1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -576,7 +576,7 @@
         <v>140</v>
       </c>
       <c r="L2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -614,7 +614,7 @@
         <v>355</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -652,7 +652,7 @@
         <v>375</v>
       </c>
       <c r="L4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -690,7 +690,7 @@
         <v>326</v>
       </c>
       <c r="L5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -728,7 +728,7 @@
         <v>315</v>
       </c>
       <c r="L6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -766,7 +766,7 @@
         <v>155</v>
       </c>
       <c r="L7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -804,7 +804,7 @@
         <v>163</v>
       </c>
       <c r="L8" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -842,7 +842,7 @@
         <v>604</v>
       </c>
       <c r="L9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -880,7 +880,7 @@
         <v>210</v>
       </c>
       <c r="L10" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -918,7 +918,7 @@
         <v>71</v>
       </c>
       <c r="L11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -956,7 +956,7 @@
         <v>58</v>
       </c>
       <c r="L12" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -994,7 +994,7 @@
         <v>122</v>
       </c>
       <c r="L13" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1032,7 +1032,7 @@
         <v>135</v>
       </c>
       <c r="L14" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1070,7 +1070,7 @@
         <v>115</v>
       </c>
       <c r="L15" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1108,7 +1108,7 @@
         <v>20</v>
       </c>
       <c r="L16" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1146,7 +1146,7 @@
         <v>465</v>
       </c>
       <c r="L17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1184,7 +1184,7 @@
         <v>45</v>
       </c>
       <c r="L18" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1222,7 +1222,7 @@
         <v>26</v>
       </c>
       <c r="L19" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1260,7 +1260,7 @@
         <v>1866</v>
       </c>
       <c r="L20" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1298,7 +1298,7 @@
         <v>59</v>
       </c>
       <c r="L21" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1336,7 +1336,7 @@
         <v>122.7</v>
       </c>
       <c r="L22" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1374,7 +1374,7 @@
         <v>125</v>
       </c>
       <c r="L23" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1412,7 +1412,7 @@
         <v>328</v>
       </c>
       <c r="L24" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1450,7 +1450,7 @@
         <v>365</v>
       </c>
       <c r="L25" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1488,7 +1488,7 @@
         <v>305</v>
       </c>
       <c r="L26" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1526,7 +1526,7 @@
         <v>300</v>
       </c>
       <c r="L27" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1564,7 +1564,7 @@
         <v>146</v>
       </c>
       <c r="L28" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1602,7 +1602,7 @@
         <v>156</v>
       </c>
       <c r="L29" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1640,7 +1640,7 @@
         <v>585</v>
       </c>
       <c r="L30" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1678,7 +1678,7 @@
         <v>199</v>
       </c>
       <c r="L31" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1716,7 +1716,7 @@
         <v>68</v>
       </c>
       <c r="L32" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1754,7 +1754,7 @@
         <v>55</v>
       </c>
       <c r="L33" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1792,7 +1792,7 @@
         <v>117</v>
       </c>
       <c r="L34" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1830,7 +1830,7 @@
         <v>124</v>
       </c>
       <c r="L35" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1868,7 +1868,7 @@
         <v>111</v>
       </c>
       <c r="L36" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1906,7 +1906,7 @@
         <v>20</v>
       </c>
       <c r="L37" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1944,7 +1944,7 @@
         <v>395</v>
       </c>
       <c r="L38" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1982,7 +1982,7 @@
         <v>41</v>
       </c>
       <c r="L39" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -2020,7 +2020,7 @@
         <v>25</v>
       </c>
       <c r="L40" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -2058,7 +2058,7 @@
         <v>1731</v>
       </c>
       <c r="L41" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -2096,7 +2096,7 @@
         <v>55</v>
       </c>
       <c r="L42" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -2134,7 +2134,7 @@
         <v>112.1</v>
       </c>
       <c r="L43" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>